<commit_message>
reporting; SUP/COMELC techs PRE from ELE; new milestoneyear spec
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NewVEDA\Veda_models\EU_TIMES_Veda2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B3FB61-F1D4-4322-A19F-ABCFC99874DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61724B2-AEB3-44EF-BCFF-E6D784BDD1A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="0" windowWidth="25110" windowHeight="15600" tabRatio="853" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3195" yWindow="3195" windowWidth="21600" windowHeight="11385" tabRatio="853" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RTT" sheetId="16" r:id="rId1"/>
@@ -139,7 +139,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3496" uniqueCount="1548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3513" uniqueCount="1553">
   <si>
     <t>FX</t>
   </si>
@@ -4776,20 +4776,35 @@
     <t>FLO~5</t>
   </si>
   <si>
-    <t>FLO~7</t>
-  </si>
-  <si>
     <t>COMPRD~1</t>
   </si>
   <si>
     <t>OBJ~1</t>
+  </si>
+  <si>
+    <t>FLO~1</t>
+  </si>
+  <si>
+    <t>msy1</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>endyear</t>
+  </si>
+  <si>
+    <t>milestoneyear</t>
+  </si>
+  <si>
+    <t>~Milestoneyears</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="33">
+  <numFmts count="29">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
@@ -4811,20 +4826,16 @@
     <numFmt numFmtId="181" formatCode="\(##\);\(##\)"/>
     <numFmt numFmtId="182" formatCode="_-[$€-2]* #,##0.00_-;\-[$€-2]* #,##0.00_-;_-[$€-2]* &quot;-&quot;??_-"/>
     <numFmt numFmtId="183" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="185" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="187" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="189" formatCode="_(&quot;£&quot;* #,##0.00_);_(&quot;£&quot;* \(#,##0.00\);_(&quot;£&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="190" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
-    <numFmt numFmtId="191" formatCode="_ &quot;kr&quot;\ * #,##0_ ;_ &quot;kr&quot;\ * \-#,##0_ ;_ &quot;kr&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="192" formatCode="_ &quot;kr&quot;\ * #,##0.00_ ;_ &quot;kr&quot;\ * \-#,##0.00_ ;_ &quot;kr&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="193" formatCode="[&gt;0.5]#,##0;[&lt;-0.5]\-#,##0;\-"/>
-    <numFmt numFmtId="194" formatCode="_-* #,##0\ &quot;F&quot;_-;\-* #,##0\ &quot;F&quot;_-;_-* &quot;-&quot;\ &quot;F&quot;_-;_-@_-"/>
-    <numFmt numFmtId="195" formatCode="_-* #,##0\ _F_-;\-* #,##0\ _F_-;_-* &quot;-&quot;\ _F_-;_-@_-"/>
-    <numFmt numFmtId="196" formatCode="_-* #,##0.00\ &quot;F&quot;_-;\-* #,##0.00\ &quot;F&quot;_-;_-* &quot;-&quot;??\ &quot;F&quot;_-;_-@_-"/>
-    <numFmt numFmtId="197" formatCode="_-* #,##0.00\ _F_-;\-* #,##0.00\ _F_-;_-* &quot;-&quot;??\ _F_-;_-@_-"/>
-    <numFmt numFmtId="198" formatCode="#,##0.0;\-#,##0.0;&quot;-&quot;"/>
+    <numFmt numFmtId="184" formatCode="_(&quot;£&quot;* #,##0.00_);_(&quot;£&quot;* \(#,##0.00\);_(&quot;£&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="185" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
+    <numFmt numFmtId="188" formatCode="[&gt;0.5]#,##0;[&lt;-0.5]\-#,##0;\-"/>
+    <numFmt numFmtId="189" formatCode="_-* #,##0\ &quot;F&quot;_-;\-* #,##0\ &quot;F&quot;_-;_-* &quot;-&quot;\ &quot;F&quot;_-;_-@_-"/>
+    <numFmt numFmtId="190" formatCode="_-* #,##0\ _F_-;\-* #,##0\ _F_-;_-* &quot;-&quot;\ _F_-;_-@_-"/>
+    <numFmt numFmtId="191" formatCode="_-* #,##0.00\ &quot;F&quot;_-;\-* #,##0.00\ &quot;F&quot;_-;_-* &quot;-&quot;??\ &quot;F&quot;_-;_-@_-"/>
+    <numFmt numFmtId="192" formatCode="_-* #,##0.00\ _F_-;\-* #,##0.00\ _F_-;_-* &quot;-&quot;??\ _F_-;_-@_-"/>
+    <numFmt numFmtId="193" formatCode="#,##0.0;\-#,##0.0;&quot;-&quot;"/>
   </numFmts>
-  <fonts count="90">
+  <fonts count="89">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -5311,10 +5322,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Helv"/>
-    </font>
-    <font>
       <sz val="8"/>
       <color indexed="9"/>
       <name val="Arial"/>
@@ -5735,7 +5742,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -6125,21 +6132,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -11562,10 +11554,10 @@
     <xf numFmtId="0" fontId="1" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="79" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="78" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="79" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="78" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="68" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -11574,7 +11566,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="83" fillId="52" borderId="0"/>
+    <xf numFmtId="0" fontId="82" fillId="52" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="55" borderId="32">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -11588,53 +11580,53 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="67" fillId="41" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="84" fillId="41" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="83" fillId="41" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="1" fontId="1" fillId="56" borderId="0"/>
-    <xf numFmtId="187" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="190" fontId="5" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="190" fontId="5" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="190" fontId="5" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="45" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="45" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="45" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="45" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="45" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="82" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="82" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="187" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="189" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="189" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="185" fontId="5" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="185" fontId="5" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="185" fontId="5" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="45" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="45" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="45" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="45" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="45" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="81" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="81" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="184" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="184" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="1" fontId="1" fillId="57" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="58" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="58" borderId="0"/>
@@ -11736,10 +11728,10 @@
     <xf numFmtId="0" fontId="70" fillId="60" borderId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="193" fontId="78" fillId="0" borderId="0">
+    <xf numFmtId="188" fontId="77" fillId="0" borderId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="193" fontId="78" fillId="0" borderId="0">
+    <xf numFmtId="188" fontId="77" fillId="0" borderId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="74" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -11750,23 +11742,23 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="85" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="80" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="84" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="79" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="85" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="85" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="85" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="86" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="195" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="197" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="194" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="196" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="84" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="84" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="84" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="85" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="190" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="192" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="189" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="191" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="82" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="82" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="82" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="81" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="81" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="81" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0"/>
@@ -11813,10 +11805,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="87" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="86" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="87" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="86" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
@@ -11844,12 +11836,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="79" fillId="31" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="79" fillId="31" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="78" fillId="31" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="78" fillId="31" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="42" borderId="30" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="42" borderId="30" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="198" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="198" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="193" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="193" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -11866,11 +11858,11 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="193" fontId="45" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="188" fontId="45" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="27" fillId="31" borderId="1"/>
-    <xf numFmtId="0" fontId="81" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="80" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
@@ -11937,11 +11929,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyProtection="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="77" fillId="54" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="76" fillId="54" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="88" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="88" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="87" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="87" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="72" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="73" fillId="61" borderId="31">
@@ -11959,7 +11951,7 @@
     <xf numFmtId="0" fontId="66" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -12001,8 +11993,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5597"/>
     <xf numFmtId="0" fontId="2" fillId="51" borderId="0" xfId="5597" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="5597" applyFont="1"/>
+    <xf numFmtId="0" fontId="88" fillId="0" borderId="0" xfId="5597" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5597" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5601">
     <cellStyle name="???????" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -19050,38 +19043,46 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="B3:I24"/>
+  <dimension ref="B3:M24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="2:9">
+    <row r="3" spans="2:13">
       <c r="B3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="2:9">
+    <row r="4" spans="2:13">
       <c r="B4">
         <v>2010</v>
       </c>
     </row>
-    <row r="7" spans="2:9">
+    <row r="7" spans="2:13">
       <c r="B7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="2:9">
+    <row r="8" spans="2:13">
       <c r="B8" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="11" spans="2:9">
+    <row r="11" spans="2:13">
       <c r="B11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="2:9">
+      <c r="L11" t="s">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13">
       <c r="B12" s="10" t="s">
         <v>42</v>
       </c>
@@ -19106,8 +19107,14 @@
       <c r="I12" s="12" t="s">
         <v>1461</v>
       </c>
-    </row>
-    <row r="13" spans="2:9">
+      <c r="L12" s="21" t="s">
+        <v>1549</v>
+      </c>
+      <c r="M12" s="10" t="s">
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13">
       <c r="B13" s="13">
         <v>1</v>
       </c>
@@ -19132,8 +19139,11 @@
       <c r="I13" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="2:9">
+      <c r="L13" t="s">
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13">
       <c r="B14" s="13">
         <v>2</v>
       </c>
@@ -19158,8 +19168,14 @@
       <c r="I14" s="13">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="2:9">
+      <c r="L14" t="s">
+        <v>1551</v>
+      </c>
+      <c r="M14">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13">
       <c r="B15" s="13">
         <v>5</v>
       </c>
@@ -19184,8 +19200,14 @@
       <c r="I15" s="13">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="2:9">
+      <c r="L15" t="s">
+        <v>1551</v>
+      </c>
+      <c r="M15">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13">
       <c r="B16" s="13">
         <v>5</v>
       </c>
@@ -19210,8 +19232,14 @@
       <c r="I16" s="13">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="2:9">
+      <c r="L16" t="s">
+        <v>1551</v>
+      </c>
+      <c r="M16">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13">
       <c r="B17" s="13">
         <v>5</v>
       </c>
@@ -19234,8 +19262,14 @@
       <c r="I17" s="13">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="2:9">
+      <c r="L17" t="s">
+        <v>1551</v>
+      </c>
+      <c r="M17">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13">
       <c r="B18" s="13">
         <v>5</v>
       </c>
@@ -19258,8 +19292,14 @@
       <c r="I18" s="13">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="2:9">
+      <c r="L18" t="s">
+        <v>1551</v>
+      </c>
+      <c r="M18">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13">
       <c r="B19" s="13">
         <v>5</v>
       </c>
@@ -19278,8 +19318,14 @@
       <c r="I19" s="13">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="2:9">
+      <c r="L19" t="s">
+        <v>1551</v>
+      </c>
+      <c r="M19">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13">
       <c r="B20" s="13">
         <v>5</v>
       </c>
@@ -19296,8 +19342,14 @@
         <v>11</v>
       </c>
       <c r="I20" s="13"/>
-    </row>
-    <row r="21" spans="2:9">
+      <c r="L20" t="s">
+        <v>1551</v>
+      </c>
+      <c r="M20">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13">
       <c r="B21" s="13">
         <v>5</v>
       </c>
@@ -19312,8 +19364,14 @@
         <v>10</v>
       </c>
       <c r="I21" s="13"/>
-    </row>
-    <row r="22" spans="2:9">
+      <c r="L21" t="s">
+        <v>1551</v>
+      </c>
+      <c r="M21">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13">
       <c r="B22" s="13">
         <v>5</v>
       </c>
@@ -19324,8 +19382,14 @@
       <c r="G22" s="13"/>
       <c r="H22" s="13"/>
       <c r="I22" s="13"/>
-    </row>
-    <row r="23" spans="2:9">
+      <c r="L22" t="s">
+        <v>1551</v>
+      </c>
+      <c r="M22">
+        <v>2045</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13">
       <c r="B23" s="13">
         <v>5</v>
       </c>
@@ -19336,8 +19400,14 @@
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
       <c r="I23" s="13"/>
-    </row>
-    <row r="24" spans="2:9">
+      <c r="L23" t="s">
+        <v>1551</v>
+      </c>
+      <c r="M23">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13">
       <c r="B24" s="13">
         <v>5</v>
       </c>
@@ -19348,6 +19418,12 @@
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
       <c r="I24" s="13"/>
+      <c r="L24" t="s">
+        <v>1551</v>
+      </c>
+      <c r="M24">
+        <v>2060</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -20258,10 +20334,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{120D8E49-1EC1-4452-8DC0-6810C7AD01E4}">
-  <dimension ref="B5:D12"/>
+  <dimension ref="B5:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -20326,7 +20402,7 @@
         <v>1541</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>1545</v>
+        <v>1547</v>
       </c>
       <c r="D10" s="17">
         <v>1</v>
@@ -20337,7 +20413,7 @@
         <v>1541</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="D11" s="17">
         <v>1</v>
@@ -20348,9 +20424,20 @@
         <v>1541</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="D12" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="B13" s="17" t="s">
+        <v>1541</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>1542</v>
+      </c>
+      <c r="D13" s="17">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updates from Wouter and preparing to run nco
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NewVEDA\Veda_models\EU_TIMES_Veda2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14CEA09E-1A14-4429-81DB-2E3C013ED37A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87F4B41-6E2C-4221-895E-46A97A83C17E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="853" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="1785" windowWidth="21600" windowHeight="11385" tabRatio="853" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RTT" sheetId="16" r:id="rId1"/>
@@ -21746,7 +21746,7 @@
   <dimension ref="B5:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -21858,7 +21858,7 @@
         <v>1550</v>
       </c>
       <c r="D14" s="22">
-        <v>1E-8</v>
+        <v>9.9999999999999995E-7</v>
       </c>
     </row>
     <row r="15" spans="2:4">
@@ -21869,7 +21869,7 @@
         <v>1549</v>
       </c>
       <c r="D15" s="22">
-        <v>1E-8</v>
+        <v>9.9999999999999995E-7</v>
       </c>
     </row>
     <row r="16" spans="2:4">
@@ -21880,7 +21880,7 @@
         <v>1551</v>
       </c>
       <c r="D16" s="22">
-        <v>1E-8</v>
+        <v>9.9999999999999995E-7</v>
       </c>
     </row>
     <row r="17" spans="2:4">
@@ -21891,7 +21891,7 @@
         <v>1552</v>
       </c>
       <c r="D17" s="22">
-        <v>1E-8</v>
+        <v>9.9999999999999995E-7</v>
       </c>
     </row>
     <row r="18" spans="2:4">

</xml_diff>